<commit_message>
Arreglat GetTransactionItem - a espera de veure si funciona
</commit_message>
<xml_diff>
--- a/Data/Output/ExtractedData.xlsx
+++ b/Data/Output/ExtractedData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovalaus-my.sharepoint.com/personal/jordi_innovalaus_com/Documents/I+D/Proves i documentació varia/Carla proves/UiPath Workflows/Calculate Client Security Hash/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovalaus-my.sharepoint.com/personal/jordi_innovalaus_com/Documents/I+D/Proves i documentació varia/Carla proves/UiPath Workflows/Calculate Client Security Hash/Data/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7B329A0F-5D1A-4F18-81DC-F4BE90387F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DBCCA6B-5D14-432C-AB3C-5A2471AE4208}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7B329A0F-5D1A-4F18-81DC-F4BE90387F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C659B13B-20AE-4212-97E1-E5AF0D8AE657}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Work Items" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,11 +339,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>